<commit_message>
First updates for PTL. Adding separate ptl product folder, and new templates for LYA and DDG VminTC. Added new headings to find and replace csv
</commit_message>
<xml_diff>
--- a/lighterFluid/inputs/demoSheet.xlsx
+++ b/lighterFluid/inputs/demoSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoghanoc\source\repos\lighterFluid\lighterFluid\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adambyrn\source\repos\lighterFluid\lighterFluid\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273F2DCC-448F-4836-9895-9B15D340D386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F95F332-8B19-443C-A916-12E1CF30D4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2220" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="templateLookup" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3092" uniqueCount="361">
   <si>
     <t>Flow</t>
   </si>
@@ -1110,6 +1110,18 @@
   </si>
   <si>
     <t>BASE::SHMOO_nom_lvl</t>
+  </si>
+  <si>
+    <t>icLya</t>
+  </si>
+  <si>
+    <t>iCLYA</t>
+  </si>
+  <si>
+    <t>ddgvmintc</t>
+  </si>
+  <si>
+    <t>VminTC</t>
   </si>
 </sst>
 </file>
@@ -2104,10 +2116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{335B2182-EA68-41EA-9EA9-384E14E7AACA}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2335,6 +2347,22 @@
         <v>349</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="B26" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="B27" t="s">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2344,7 +2372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB20E6F1-DE4C-470B-9A99-FCCB71C10BDB}">
   <dimension ref="A1:AU61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="AL5" sqref="AL5"/>
@@ -23068,15 +23096,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002200735434F8BC4E847E79EE962A8A4A" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="83f675189dd244c3c7bcfe6ef2723be5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1cd8a145-0748-4d97-9311-a3be7d9cf841" xmlns:ns3="2e84272e-479a-4b4f-8918-ffe580143f91" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3dd33d4618ec6cc7e4782be4e466c7bd" ns2:_="" ns3:_="">
     <xsd:import namespace="1cd8a145-0748-4d97-9311-a3be7d9cf841"/>
@@ -23253,15 +23272,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D30E43E-9BCC-44E6-A6FA-8336DBB02DA4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BD6ABBF-3907-430F-A89A-B3039F113893}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23278,4 +23298,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D30E43E-9BCC-44E6-A6FA-8336DBB02DA4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>